<commit_message>
upload experiment low and high
</commit_message>
<xml_diff>
--- a/Compare_SOTA.xlsx
+++ b/Compare_SOTA.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive - Hanoi University of Science and Technology\Desktop\AGF_IVIF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED347A-0BBB-4A92-8FB5-5EF919CF7158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{7E3F11DC-7DEA-4982-B14A-0AB0C0AB0965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5CA58A07-28D8-4F6F-8CC7-75009E77A9A1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{5CA58A07-28D8-4F6F-8CC7-75009E77A9A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SOTA" sheetId="1" r:id="rId1"/>
+    <sheet name="Low" sheetId="3" r:id="rId2"/>
+    <sheet name="High" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
   <si>
     <t>BTSFusion</t>
   </si>
@@ -115,11 +118,47 @@
   <si>
     <t>PFCFuse</t>
   </si>
+  <si>
+    <t>Low_1</t>
+  </si>
+  <si>
+    <t>Low_2</t>
+  </si>
+  <si>
+    <t>Low_3</t>
+  </si>
+  <si>
+    <t>Low_4</t>
+  </si>
+  <si>
+    <t>Low_5</t>
+  </si>
+  <si>
+    <t>Low_6</t>
+  </si>
+  <si>
+    <t>High_1</t>
+  </si>
+  <si>
+    <t>High_2</t>
+  </si>
+  <si>
+    <t>High_3</t>
+  </si>
+  <si>
+    <t>High_4</t>
+  </si>
+  <si>
+    <t>High_5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -440,11 +479,606 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1365,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D96C6E2-4670-4300-89EE-FC1DB529284B}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2432,144 +3066,1103 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C12">
-    <cfRule type="top10" dxfId="83" priority="84" rank="3"/>
-    <cfRule type="top10" dxfId="82" priority="83" rank="2"/>
-    <cfRule type="top10" dxfId="81" priority="82" rank="1"/>
+    <cfRule type="top10" dxfId="167" priority="84" rank="3"/>
+    <cfRule type="top10" dxfId="166" priority="83" rank="2"/>
+    <cfRule type="top10" dxfId="165" priority="82" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C24">
-    <cfRule type="top10" dxfId="80" priority="45" rank="3"/>
-    <cfRule type="top10" dxfId="79" priority="44" rank="2"/>
-    <cfRule type="top10" dxfId="78" priority="43" rank="1"/>
+    <cfRule type="top10" dxfId="164" priority="45" rank="3"/>
+    <cfRule type="top10" dxfId="163" priority="44" rank="2"/>
+    <cfRule type="top10" dxfId="162" priority="43" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D12">
-    <cfRule type="top10" dxfId="77" priority="81" rank="3"/>
-    <cfRule type="top10" dxfId="76" priority="80" rank="2"/>
-    <cfRule type="top10" dxfId="75" priority="79" rank="1"/>
+    <cfRule type="top10" dxfId="161" priority="81" rank="3"/>
+    <cfRule type="top10" dxfId="160" priority="80" rank="2"/>
+    <cfRule type="top10" dxfId="159" priority="79" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D24">
-    <cfRule type="top10" dxfId="74" priority="41" rank="2"/>
-    <cfRule type="top10" dxfId="73" priority="42" rank="3"/>
-    <cfRule type="top10" dxfId="72" priority="40" rank="1"/>
+    <cfRule type="top10" dxfId="158" priority="41" rank="2"/>
+    <cfRule type="top10" dxfId="157" priority="42" rank="3"/>
+    <cfRule type="top10" dxfId="156" priority="40" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E12">
-    <cfRule type="top10" dxfId="71" priority="78" rank="3"/>
-    <cfRule type="top10" dxfId="70" priority="77" rank="2"/>
-    <cfRule type="top10" dxfId="69" priority="76" rank="1"/>
+    <cfRule type="top10" dxfId="155" priority="78" rank="3"/>
+    <cfRule type="top10" dxfId="154" priority="77" rank="2"/>
+    <cfRule type="top10" dxfId="153" priority="76" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E24">
-    <cfRule type="top10" dxfId="68" priority="37" rank="1"/>
-    <cfRule type="top10" dxfId="67" priority="38" rank="2"/>
-    <cfRule type="top10" dxfId="66" priority="39" rank="3"/>
+    <cfRule type="top10" dxfId="152" priority="37" rank="1"/>
+    <cfRule type="top10" dxfId="151" priority="38" rank="2"/>
+    <cfRule type="top10" dxfId="150" priority="39" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F12">
-    <cfRule type="top10" dxfId="65" priority="74" rank="2"/>
-    <cfRule type="top10" dxfId="64" priority="75" rank="3"/>
-    <cfRule type="top10" dxfId="63" priority="73" rank="1"/>
+    <cfRule type="top10" dxfId="149" priority="74" rank="2"/>
+    <cfRule type="top10" dxfId="148" priority="75" rank="3"/>
+    <cfRule type="top10" dxfId="147" priority="73" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:F24">
-    <cfRule type="top10" dxfId="62" priority="34" rank="1"/>
-    <cfRule type="top10" dxfId="61" priority="35" rank="2"/>
-    <cfRule type="top10" dxfId="60" priority="36" rank="3"/>
+    <cfRule type="top10" dxfId="146" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="145" priority="35" rank="2"/>
+    <cfRule type="top10" dxfId="144" priority="36" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G12">
-    <cfRule type="top10" dxfId="59" priority="72" rank="3"/>
-    <cfRule type="top10" dxfId="58" priority="71" rank="2"/>
-    <cfRule type="top10" dxfId="57" priority="70" rank="1"/>
+    <cfRule type="top10" dxfId="143" priority="72" rank="3"/>
+    <cfRule type="top10" dxfId="142" priority="71" rank="2"/>
+    <cfRule type="top10" dxfId="141" priority="70" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:G24">
-    <cfRule type="top10" dxfId="56" priority="33" rank="3"/>
-    <cfRule type="top10" dxfId="55" priority="31" rank="1"/>
-    <cfRule type="top10" dxfId="54" priority="32" rank="2"/>
+    <cfRule type="top10" dxfId="140" priority="33" rank="3"/>
+    <cfRule type="top10" dxfId="139" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="138" priority="32" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H12">
-    <cfRule type="top10" dxfId="53" priority="69" rank="3"/>
-    <cfRule type="top10" dxfId="52" priority="68" rank="2"/>
-    <cfRule type="top10" dxfId="51" priority="67" rank="1"/>
+    <cfRule type="top10" dxfId="137" priority="69" rank="3"/>
+    <cfRule type="top10" dxfId="136" priority="68" rank="2"/>
+    <cfRule type="top10" dxfId="135" priority="67" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H24">
-    <cfRule type="top10" dxfId="50" priority="28" rank="1"/>
-    <cfRule type="top10" dxfId="49" priority="30" rank="3"/>
-    <cfRule type="top10" dxfId="48" priority="29" rank="2"/>
+    <cfRule type="top10" dxfId="134" priority="28" rank="1"/>
+    <cfRule type="top10" dxfId="133" priority="30" rank="3"/>
+    <cfRule type="top10" dxfId="132" priority="29" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I12">
-    <cfRule type="top10" dxfId="47" priority="66" rank="3"/>
-    <cfRule type="top10" dxfId="46" priority="65" rank="2"/>
-    <cfRule type="top10" dxfId="45" priority="64" rank="1"/>
+    <cfRule type="top10" dxfId="131" priority="66" rank="3"/>
+    <cfRule type="top10" dxfId="130" priority="65" rank="2"/>
+    <cfRule type="top10" dxfId="129" priority="64" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I24">
-    <cfRule type="top10" dxfId="44" priority="25" rank="1"/>
-    <cfRule type="top10" dxfId="43" priority="26" rank="2"/>
-    <cfRule type="top10" dxfId="42" priority="27" rank="3"/>
+    <cfRule type="top10" dxfId="128" priority="25" rank="1"/>
+    <cfRule type="top10" dxfId="127" priority="26" rank="2"/>
+    <cfRule type="top10" dxfId="126" priority="27" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J12">
-    <cfRule type="top10" dxfId="41" priority="63" rank="3"/>
-    <cfRule type="top10" dxfId="40" priority="62" rank="2"/>
-    <cfRule type="top10" dxfId="39" priority="61" rank="1"/>
+    <cfRule type="top10" dxfId="125" priority="63" rank="3"/>
+    <cfRule type="top10" dxfId="124" priority="62" rank="2"/>
+    <cfRule type="top10" dxfId="123" priority="61" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J24">
-    <cfRule type="top10" dxfId="38" priority="22" rank="1"/>
-    <cfRule type="top10" dxfId="37" priority="23" rank="2"/>
-    <cfRule type="top10" dxfId="36" priority="24" rank="3"/>
+    <cfRule type="top10" dxfId="122" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="121" priority="23" rank="2"/>
+    <cfRule type="top10" dxfId="120" priority="24" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="top10" dxfId="35" priority="58" rank="1"/>
-    <cfRule type="top10" dxfId="34" priority="59" rank="2"/>
-    <cfRule type="top10" dxfId="33" priority="60" rank="3"/>
+    <cfRule type="top10" dxfId="119" priority="58" rank="1"/>
+    <cfRule type="top10" dxfId="118" priority="59" rank="2"/>
+    <cfRule type="top10" dxfId="117" priority="60" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K24">
-    <cfRule type="top10" dxfId="32" priority="21" rank="3"/>
-    <cfRule type="top10" dxfId="31" priority="19" rank="1"/>
-    <cfRule type="top10" dxfId="30" priority="20" rank="2"/>
+    <cfRule type="top10" dxfId="116" priority="21" rank="3"/>
+    <cfRule type="top10" dxfId="115" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="114" priority="20" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L12">
-    <cfRule type="top10" dxfId="29" priority="4" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="28" priority="5" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="27" priority="6" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="113" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="112" priority="5" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="111" priority="6" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L24">
-    <cfRule type="top10" dxfId="26" priority="2" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="25" priority="3" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="24" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="110" priority="2" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="109" priority="3" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="108" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M12">
-    <cfRule type="top10" dxfId="23" priority="57" rank="3"/>
-    <cfRule type="top10" dxfId="22" priority="56" rank="2"/>
-    <cfRule type="top10" dxfId="21" priority="55" rank="1"/>
+    <cfRule type="top10" dxfId="107" priority="57" rank="3"/>
+    <cfRule type="top10" dxfId="106" priority="56" rank="2"/>
+    <cfRule type="top10" dxfId="105" priority="55" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16:M24">
-    <cfRule type="top10" dxfId="20" priority="18" rank="3"/>
-    <cfRule type="top10" dxfId="19" priority="17" rank="2"/>
-    <cfRule type="top10" dxfId="18" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="104" priority="18" rank="3"/>
+    <cfRule type="top10" dxfId="103" priority="17" rank="2"/>
+    <cfRule type="top10" dxfId="102" priority="16" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N12">
-    <cfRule type="top10" dxfId="17" priority="52" rank="1"/>
-    <cfRule type="top10" dxfId="16" priority="54" rank="3"/>
-    <cfRule type="top10" dxfId="15" priority="53" rank="2"/>
+    <cfRule type="top10" dxfId="101" priority="52" rank="1"/>
+    <cfRule type="top10" dxfId="100" priority="54" rank="3"/>
+    <cfRule type="top10" dxfId="99" priority="53" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:N24">
-    <cfRule type="top10" dxfId="14" priority="13" rank="1"/>
-    <cfRule type="top10" dxfId="13" priority="14" rank="2"/>
-    <cfRule type="top10" dxfId="12" priority="15" rank="3"/>
+    <cfRule type="top10" dxfId="98" priority="13" rank="1"/>
+    <cfRule type="top10" dxfId="97" priority="14" rank="2"/>
+    <cfRule type="top10" dxfId="96" priority="15" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P12">
-    <cfRule type="top10" dxfId="11" priority="51" rank="3"/>
-    <cfRule type="top10" dxfId="10" priority="49" rank="1"/>
-    <cfRule type="top10" dxfId="9" priority="50" rank="2"/>
+    <cfRule type="top10" dxfId="95" priority="51" rank="3"/>
+    <cfRule type="top10" dxfId="94" priority="49" rank="1"/>
+    <cfRule type="top10" dxfId="93" priority="50" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P24">
-    <cfRule type="top10" dxfId="8" priority="10" rank="1"/>
-    <cfRule type="top10" dxfId="7" priority="12" rank="3"/>
-    <cfRule type="top10" dxfId="6" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="92" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="91" priority="12" rank="3"/>
+    <cfRule type="top10" dxfId="90" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q12">
-    <cfRule type="top10" dxfId="5" priority="48" rank="3"/>
-    <cfRule type="top10" dxfId="4" priority="47" rank="2"/>
-    <cfRule type="top10" dxfId="3" priority="46" rank="1"/>
+    <cfRule type="top10" dxfId="89" priority="48" rank="3"/>
+    <cfRule type="top10" dxfId="88" priority="47" rank="2"/>
+    <cfRule type="top10" dxfId="87" priority="46" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16:Q24">
-    <cfRule type="top10" dxfId="2" priority="8" rank="2"/>
-    <cfRule type="top10" dxfId="1" priority="9" rank="3"/>
-    <cfRule type="top10" dxfId="0" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="86" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="85" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="84" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658708F2-6B47-4C8E-89C7-B435A839B89F}">
+  <dimension ref="A2:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26">
+        <v>6.8735258124999996</v>
+      </c>
+      <c r="D5" s="27">
+        <v>4.0713164499999994</v>
+      </c>
+      <c r="E5" s="27">
+        <v>12.557768637500001</v>
+      </c>
+      <c r="F5" s="27">
+        <v>4.1091918875000006</v>
+      </c>
+      <c r="G5" s="27">
+        <v>49.267256699999997</v>
+      </c>
+      <c r="H5" s="27">
+        <v>75.481208801269531</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.58151787519454956</v>
+      </c>
+      <c r="J5" s="27">
+        <v>1.515410900115967</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0.98291439999999997</v>
+      </c>
+      <c r="L5" s="27">
+        <v>5.4024599999999999E-2</v>
+      </c>
+      <c r="M5" s="27">
+        <v>62.4993814125</v>
+      </c>
+      <c r="N5" s="27">
+        <v>0.70679438750000001</v>
+      </c>
+      <c r="O5" s="27">
+        <v>1.9508975000000001E-2</v>
+      </c>
+      <c r="P5" s="27">
+        <v>0.46041969999999999</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>0.50340401250000011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="29">
+        <v>6.1697057375000002</v>
+      </c>
+      <c r="D6" s="29">
+        <v>2.3266108750000001</v>
+      </c>
+      <c r="E6" s="29">
+        <v>9.218897912500001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>3.2531189875000002</v>
+      </c>
+      <c r="G6" s="29">
+        <v>26.711977300000001</v>
+      </c>
+      <c r="H6" s="29">
+        <v>44.698509216308587</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0.64546197652816772</v>
+      </c>
+      <c r="J6" s="29">
+        <v>1.2687408924102781</v>
+      </c>
+      <c r="K6" s="29">
+        <v>0.77071727499999998</v>
+      </c>
+      <c r="L6" s="29">
+        <v>2.4184037500000002E-2</v>
+      </c>
+      <c r="M6" s="29">
+        <v>65.914170900000002</v>
+      </c>
+      <c r="N6" s="29">
+        <v>0.58419960000000004</v>
+      </c>
+      <c r="O6" s="29">
+        <v>4.0069499999999996E-3</v>
+      </c>
+      <c r="P6" s="29">
+        <v>0.42773987499999999</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0.49829816249999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="18"/>
+      <c r="B7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="29">
+        <v>6.7950501375000014</v>
+      </c>
+      <c r="D7" s="29">
+        <v>5.3517875125000014</v>
+      </c>
+      <c r="E7" s="29">
+        <v>12.129406012500001</v>
+      </c>
+      <c r="F7" s="29">
+        <v>3.9979591750000001</v>
+      </c>
+      <c r="G7" s="29">
+        <v>47.095998512500003</v>
+      </c>
+      <c r="H7" s="29">
+        <v>72.203582763671875</v>
+      </c>
+      <c r="I7" s="29">
+        <v>0.59926795959472656</v>
+      </c>
+      <c r="J7" s="29">
+        <v>1.6870254278182979</v>
+      </c>
+      <c r="K7" s="29">
+        <v>0.99955040000000006</v>
+      </c>
+      <c r="L7" s="29">
+        <v>4.7768412500000003E-2</v>
+      </c>
+      <c r="M7" s="29">
+        <v>62.975000000000001</v>
+      </c>
+      <c r="N7" s="29">
+        <v>0.7139308875</v>
+      </c>
+      <c r="O7" s="29">
+        <v>6.4379124999999994E-3</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0.46322533750000011</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0.51005310000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="29">
+        <v>6.7948362500000004</v>
+      </c>
+      <c r="D8" s="29">
+        <v>5.3567328750000014</v>
+      </c>
+      <c r="E8" s="29">
+        <v>12.1862954625</v>
+      </c>
+      <c r="F8" s="29">
+        <v>4.0024630999999999</v>
+      </c>
+      <c r="G8" s="29">
+        <v>47.100811512500002</v>
+      </c>
+      <c r="H8" s="29">
+        <v>72.189552307128906</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.59905439615249634</v>
+      </c>
+      <c r="J8" s="29">
+        <v>1.6850211620330811</v>
+      </c>
+      <c r="K8" s="29">
+        <v>0.99861033749999994</v>
+      </c>
+      <c r="L8" s="29">
+        <v>4.7767012499999997E-2</v>
+      </c>
+      <c r="M8" s="29">
+        <v>62.975348612500007</v>
+      </c>
+      <c r="N8" s="29">
+        <v>0.71328571250000006</v>
+      </c>
+      <c r="O8" s="29">
+        <v>6.6479125000000003E-3</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0.46315044999999999</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>0.51001948749999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="29">
+        <v>6.2440859624999998</v>
+      </c>
+      <c r="D9" s="29">
+        <v>2.7355148749999998</v>
+      </c>
+      <c r="E9" s="29">
+        <v>11.238335475</v>
+      </c>
+      <c r="F9" s="29">
+        <v>3.6020286750000001</v>
+      </c>
+      <c r="G9" s="29">
+        <v>38.586125849999988</v>
+      </c>
+      <c r="H9" s="29">
+        <v>40.909221649169922</v>
+      </c>
+      <c r="I9" s="29">
+        <v>0.62420332431793213</v>
+      </c>
+      <c r="J9" s="29">
+        <v>1.51038122177124</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0.82893146249999994</v>
+      </c>
+      <c r="L9" s="29">
+        <v>3.11991E-2</v>
+      </c>
+      <c r="M9" s="29">
+        <v>64.610473924999994</v>
+      </c>
+      <c r="N9" s="29">
+        <v>0.63639513749999987</v>
+      </c>
+      <c r="O9" s="29">
+        <v>1.0807325E-2</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.40310208749999998</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>0.49732243749999988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="18"/>
+      <c r="B10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="29">
+        <v>6.3481880500000001</v>
+      </c>
+      <c r="D10" s="29">
+        <v>2.6505951625000002</v>
+      </c>
+      <c r="E10" s="29">
+        <v>11.4472860375</v>
+      </c>
+      <c r="F10" s="29">
+        <v>3.6997698125</v>
+      </c>
+      <c r="G10" s="29">
+        <v>39.604275862500003</v>
+      </c>
+      <c r="H10" s="29">
+        <v>50.349334716796882</v>
+      </c>
+      <c r="I10" s="29">
+        <v>0.61574745178222656</v>
+      </c>
+      <c r="J10" s="29">
+        <v>1.4905151128768921</v>
+      </c>
+      <c r="K10" s="29">
+        <v>0.82536721250000011</v>
+      </c>
+      <c r="L10" s="29">
+        <v>2.98666E-2</v>
+      </c>
+      <c r="M10" s="29">
+        <v>64.935572287500008</v>
+      </c>
+      <c r="N10" s="29">
+        <v>0.66110541249999999</v>
+      </c>
+      <c r="O10" s="29">
+        <v>1.022E-2</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0.43854524999999989</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>0.5098085</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="18"/>
+      <c r="B11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="31">
+        <v>6.7948178124999998</v>
+      </c>
+      <c r="D11" s="31">
+        <v>5.356986225</v>
+      </c>
+      <c r="E11" s="31">
+        <v>12.194338112500001</v>
+      </c>
+      <c r="F11" s="31">
+        <v>4.0033985625000001</v>
+      </c>
+      <c r="G11" s="31">
+        <v>47.101428187499991</v>
+      </c>
+      <c r="H11" s="31">
+        <v>72.187301635742188</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0.59901273250579834</v>
+      </c>
+      <c r="J11" s="31">
+        <v>1.6846176385879521</v>
+      </c>
+      <c r="K11" s="31">
+        <v>0.99851741250000003</v>
+      </c>
+      <c r="L11" s="31">
+        <v>4.7766875000000007E-2</v>
+      </c>
+      <c r="M11" s="31">
+        <v>62.975375062500007</v>
+      </c>
+      <c r="N11" s="31">
+        <v>0.71323686249999996</v>
+      </c>
+      <c r="O11" s="31">
+        <v>6.6902625000000004E-3</v>
+      </c>
+      <c r="P11" s="31">
+        <v>0.46313433749999999</v>
+      </c>
+      <c r="Q11" s="32">
+        <v>0.5100095</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C5:C11">
+    <cfRule type="top10" dxfId="83" priority="85" rank="1"/>
+    <cfRule type="top10" dxfId="82" priority="86" rank="2"/>
+    <cfRule type="top10" dxfId="81" priority="87" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D11">
+    <cfRule type="top10" dxfId="80" priority="88" rank="1"/>
+    <cfRule type="top10" dxfId="79" priority="89" rank="2"/>
+    <cfRule type="top10" dxfId="78" priority="90" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E11">
+    <cfRule type="top10" dxfId="77" priority="91" rank="1"/>
+    <cfRule type="top10" dxfId="76" priority="92" rank="2"/>
+    <cfRule type="top10" dxfId="75" priority="93" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F11">
+    <cfRule type="top10" dxfId="74" priority="94" rank="1"/>
+    <cfRule type="top10" dxfId="73" priority="95" rank="2"/>
+    <cfRule type="top10" dxfId="72" priority="96" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G11">
+    <cfRule type="top10" dxfId="71" priority="97" rank="1"/>
+    <cfRule type="top10" dxfId="70" priority="98" rank="2"/>
+    <cfRule type="top10" dxfId="69" priority="99" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H11">
+    <cfRule type="top10" dxfId="68" priority="100" rank="1"/>
+    <cfRule type="top10" dxfId="67" priority="101" rank="2"/>
+    <cfRule type="top10" dxfId="66" priority="102" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I11">
+    <cfRule type="top10" dxfId="65" priority="103" rank="1"/>
+    <cfRule type="top10" dxfId="64" priority="104" rank="2"/>
+    <cfRule type="top10" dxfId="63" priority="105" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J11">
+    <cfRule type="top10" dxfId="62" priority="106" rank="1"/>
+    <cfRule type="top10" dxfId="61" priority="107" rank="2"/>
+    <cfRule type="top10" dxfId="60" priority="108" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K11">
+    <cfRule type="top10" dxfId="59" priority="109" rank="1"/>
+    <cfRule type="top10" dxfId="58" priority="110" rank="2"/>
+    <cfRule type="top10" dxfId="57" priority="111" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:L11">
+    <cfRule type="top10" dxfId="56" priority="112" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="55" priority="113" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="54" priority="114" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M11">
+    <cfRule type="top10" dxfId="53" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="116" rank="2"/>
+    <cfRule type="top10" dxfId="51" priority="117" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:N11">
+    <cfRule type="top10" dxfId="50" priority="118" rank="1"/>
+    <cfRule type="top10" dxfId="49" priority="119" rank="2"/>
+    <cfRule type="top10" dxfId="48" priority="120" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P11">
+    <cfRule type="top10" dxfId="47" priority="121" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="122" rank="2"/>
+    <cfRule type="top10" dxfId="45" priority="123" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5:Q11">
+    <cfRule type="top10" dxfId="44" priority="124" rank="1"/>
+    <cfRule type="top10" dxfId="43" priority="125" rank="2"/>
+    <cfRule type="top10" dxfId="42" priority="126" rank="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E82DCF-ACB4-4573-B551-26FEF839147A}">
+  <dimension ref="A2:Q10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26">
+        <v>6.8735258124999996</v>
+      </c>
+      <c r="D5" s="27">
+        <v>4.0713164499999994</v>
+      </c>
+      <c r="E5" s="27">
+        <v>12.557768637500001</v>
+      </c>
+      <c r="F5" s="27">
+        <v>4.1091918875000006</v>
+      </c>
+      <c r="G5" s="27">
+        <v>49.267256699999997</v>
+      </c>
+      <c r="H5" s="27">
+        <v>75.481208801269531</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.58151787519454956</v>
+      </c>
+      <c r="J5" s="27">
+        <v>1.515410900115967</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0.98291439999999997</v>
+      </c>
+      <c r="L5" s="27">
+        <v>5.4024599999999999E-2</v>
+      </c>
+      <c r="M5" s="27">
+        <v>62.4993814125</v>
+      </c>
+      <c r="N5" s="27">
+        <v>0.70679438750000001</v>
+      </c>
+      <c r="O5" s="27">
+        <v>1.9508975000000001E-2</v>
+      </c>
+      <c r="P5" s="27">
+        <v>0.46041969999999999</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>0.50340401250000011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="29">
+        <v>6.1697057375000002</v>
+      </c>
+      <c r="D6" s="29">
+        <v>2.3266108750000001</v>
+      </c>
+      <c r="E6" s="29">
+        <v>9.218897912500001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>3.2531189875000002</v>
+      </c>
+      <c r="G6" s="29">
+        <v>26.711977300000001</v>
+      </c>
+      <c r="H6" s="29">
+        <v>44.698509216308587</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0.64546197652816772</v>
+      </c>
+      <c r="J6" s="29">
+        <v>1.2687408924102781</v>
+      </c>
+      <c r="K6" s="29">
+        <v>0.77071727499999998</v>
+      </c>
+      <c r="L6" s="29">
+        <v>2.4184037500000002E-2</v>
+      </c>
+      <c r="M6" s="29">
+        <v>65.914170900000002</v>
+      </c>
+      <c r="N6" s="29">
+        <v>0.58419960000000004</v>
+      </c>
+      <c r="O6" s="29">
+        <v>4.0069499999999996E-3</v>
+      </c>
+      <c r="P6" s="29">
+        <v>0.42773987499999999</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0.49829816249999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="18"/>
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="29">
+        <v>6.7950501375000014</v>
+      </c>
+      <c r="D7" s="29">
+        <v>5.3517875125000014</v>
+      </c>
+      <c r="E7" s="29">
+        <v>12.129406012500001</v>
+      </c>
+      <c r="F7" s="29">
+        <v>3.9979591750000001</v>
+      </c>
+      <c r="G7" s="29">
+        <v>47.095998512500003</v>
+      </c>
+      <c r="H7" s="29">
+        <v>72.203582763671875</v>
+      </c>
+      <c r="I7" s="29">
+        <v>0.59926795959472656</v>
+      </c>
+      <c r="J7" s="29">
+        <v>1.6870254278182979</v>
+      </c>
+      <c r="K7" s="29">
+        <v>0.99955040000000006</v>
+      </c>
+      <c r="L7" s="29">
+        <v>4.7768412500000003E-2</v>
+      </c>
+      <c r="M7" s="29">
+        <v>62.975000000000001</v>
+      </c>
+      <c r="N7" s="29">
+        <v>0.7139308875</v>
+      </c>
+      <c r="O7" s="29">
+        <v>6.4379124999999994E-3</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0.46322533750000011</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0.51005310000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="29">
+        <v>6.7948362500000004</v>
+      </c>
+      <c r="D8" s="29">
+        <v>5.3567328750000014</v>
+      </c>
+      <c r="E8" s="29">
+        <v>12.1862954625</v>
+      </c>
+      <c r="F8" s="29">
+        <v>4.0024630999999999</v>
+      </c>
+      <c r="G8" s="29">
+        <v>47.100811512500002</v>
+      </c>
+      <c r="H8" s="29">
+        <v>72.189552307128906</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.59905439615249634</v>
+      </c>
+      <c r="J8" s="29">
+        <v>1.6850211620330811</v>
+      </c>
+      <c r="K8" s="29">
+        <v>0.99861033749999994</v>
+      </c>
+      <c r="L8" s="29">
+        <v>4.7767012499999997E-2</v>
+      </c>
+      <c r="M8" s="29">
+        <v>62.975348612500007</v>
+      </c>
+      <c r="N8" s="29">
+        <v>0.71328571250000006</v>
+      </c>
+      <c r="O8" s="29">
+        <v>6.6479125000000003E-3</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0.46315044999999999</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>0.51001948749999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="29">
+        <v>6.2440859624999998</v>
+      </c>
+      <c r="D9" s="29">
+        <v>2.7355148749999998</v>
+      </c>
+      <c r="E9" s="29">
+        <v>11.238335475</v>
+      </c>
+      <c r="F9" s="29">
+        <v>3.6020286750000001</v>
+      </c>
+      <c r="G9" s="29">
+        <v>38.586125849999988</v>
+      </c>
+      <c r="H9" s="29">
+        <v>40.909221649169922</v>
+      </c>
+      <c r="I9" s="29">
+        <v>0.62420332431793213</v>
+      </c>
+      <c r="J9" s="29">
+        <v>1.51038122177124</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0.82893146249999994</v>
+      </c>
+      <c r="L9" s="29">
+        <v>3.11991E-2</v>
+      </c>
+      <c r="M9" s="29">
+        <v>64.610473924999994</v>
+      </c>
+      <c r="N9" s="29">
+        <v>0.63639513749999987</v>
+      </c>
+      <c r="O9" s="29">
+        <v>1.0807325E-2</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.40310208749999998</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>0.49732243749999988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="18"/>
+      <c r="B10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="31">
+        <v>6.3481880500000001</v>
+      </c>
+      <c r="D10" s="31">
+        <v>2.6505951625000002</v>
+      </c>
+      <c r="E10" s="31">
+        <v>11.4472860375</v>
+      </c>
+      <c r="F10" s="31">
+        <v>3.6997698125</v>
+      </c>
+      <c r="G10" s="31">
+        <v>39.604275862500003</v>
+      </c>
+      <c r="H10" s="31">
+        <v>50.349334716796882</v>
+      </c>
+      <c r="I10" s="31">
+        <v>0.61574745178222656</v>
+      </c>
+      <c r="J10" s="31">
+        <v>1.4905151128768921</v>
+      </c>
+      <c r="K10" s="31">
+        <v>0.82536721250000011</v>
+      </c>
+      <c r="L10" s="31">
+        <v>2.98666E-2</v>
+      </c>
+      <c r="M10" s="31">
+        <v>64.935572287500008</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0.66110541249999999</v>
+      </c>
+      <c r="O10" s="31">
+        <v>1.022E-2</v>
+      </c>
+      <c r="P10" s="31">
+        <v>0.43854524999999989</v>
+      </c>
+      <c r="Q10" s="32">
+        <v>0.5098085</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C5:C10">
+    <cfRule type="top10" dxfId="41" priority="127" rank="1"/>
+    <cfRule type="top10" dxfId="40" priority="128" rank="2"/>
+    <cfRule type="top10" dxfId="39" priority="129" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D10">
+    <cfRule type="top10" dxfId="38" priority="130" rank="1"/>
+    <cfRule type="top10" dxfId="37" priority="131" rank="2"/>
+    <cfRule type="top10" dxfId="36" priority="132" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E10">
+    <cfRule type="top10" dxfId="35" priority="133" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="134" rank="2"/>
+    <cfRule type="top10" dxfId="33" priority="135" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F10">
+    <cfRule type="top10" dxfId="32" priority="136" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="137" rank="2"/>
+    <cfRule type="top10" dxfId="30" priority="138" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G10">
+    <cfRule type="top10" dxfId="29" priority="139" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="140" rank="2"/>
+    <cfRule type="top10" dxfId="27" priority="141" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H10">
+    <cfRule type="top10" dxfId="26" priority="142" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="143" rank="2"/>
+    <cfRule type="top10" dxfId="24" priority="144" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I10">
+    <cfRule type="top10" dxfId="23" priority="145" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="146" rank="2"/>
+    <cfRule type="top10" dxfId="21" priority="147" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J10">
+    <cfRule type="top10" dxfId="20" priority="148" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="149" rank="2"/>
+    <cfRule type="top10" dxfId="18" priority="150" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K10">
+    <cfRule type="top10" dxfId="17" priority="151" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="152" rank="2"/>
+    <cfRule type="top10" dxfId="15" priority="153" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:L10">
+    <cfRule type="top10" dxfId="14" priority="154" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="155" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="12" priority="156" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M10">
+    <cfRule type="top10" dxfId="11" priority="157" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="158" rank="2"/>
+    <cfRule type="top10" dxfId="9" priority="159" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:N10">
+    <cfRule type="top10" dxfId="8" priority="160" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="161" rank="2"/>
+    <cfRule type="top10" dxfId="6" priority="162" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P10">
+    <cfRule type="top10" dxfId="5" priority="163" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="164" rank="2"/>
+    <cfRule type="top10" dxfId="3" priority="165" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5:Q10">
+    <cfRule type="top10" dxfId="2" priority="166" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="167" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="168" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change fusion detail with MLE
</commit_message>
<xml_diff>
--- a/Compare_SOTA.xlsx
+++ b/Compare_SOTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive - Hanoi University of Science and Technology\Desktop\AGF_IVIF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F971F-BE1F-4217-922B-5898DCA29002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DEF34C-A19C-4211-8390-46A58E91AC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{5CA58A07-28D8-4F6F-8CC7-75009E77A9A1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5CA58A07-28D8-4F6F-8CC7-75009E77A9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="SOTA" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
   <si>
     <t>BTSFusion</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>High_5</t>
+  </si>
+  <si>
+    <t>High_6</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -488,15 +491,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2262,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D96C6E2-4670-4300-89EE-FC1DB529284B}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3476,15 +3474,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380993AB-99C4-4562-816B-79B0619A1C10}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="38"/>
-    <col min="2" max="2" width="12.6328125" style="38" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="38"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3547,16 +3543,16 @@
       <c r="C5" s="4">
         <v>6.3889125875000001</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5">
         <v>2.3609583125000002</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5">
         <v>36.939847212499998</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5">
         <v>61.939380645751953</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5">
         <v>0.5588606625000001</v>
       </c>
       <c r="H5" s="5">
@@ -3573,16 +3569,16 @@
       <c r="C6" s="4">
         <v>6.6193734624999996</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6">
         <v>3.3290330875</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6">
         <v>40.583932037499999</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6">
         <v>68.403762817382813</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6">
         <v>0.8609181749999999</v>
       </c>
       <c r="H6" s="5">
@@ -3599,16 +3595,16 @@
       <c r="C7" s="4">
         <v>6.7883752624999998</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7">
         <v>5.4795075999999998</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7">
         <v>47.763012687499987</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7">
         <v>70.065147399902344</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7">
         <v>1.0558631375</v>
       </c>
       <c r="H7" s="5">
@@ -3625,16 +3621,16 @@
       <c r="C8" s="4">
         <v>6.6655957624999997</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8">
         <v>2.2488896</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8">
         <v>41.741178162499999</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8">
         <v>52.65240478515625</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8">
         <v>0.74008070000000004</v>
       </c>
       <c r="H8" s="5">
@@ -3651,16 +3647,16 @@
       <c r="C9" s="4">
         <v>6.7190941249999998</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9">
         <v>2.4238344000000001</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9">
         <v>42.906301775000003</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9">
         <v>64.048255920410156</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9">
         <v>0.678054975</v>
       </c>
       <c r="H9" s="5">
@@ -3677,16 +3673,16 @@
       <c r="C10" s="4">
         <v>6.3960395999999999</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10">
         <v>2.3877774500000002</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10">
         <v>35.829575237500002</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10">
         <v>54.317493438720703</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10">
         <v>0.84554296250000005</v>
       </c>
       <c r="H10" s="5">
@@ -3703,16 +3699,16 @@
       <c r="C11" s="4">
         <v>6.3098833624999999</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11">
         <v>3.805171375</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11">
         <v>43.552553550000013</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11">
         <v>64.554885864257813</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11">
         <v>0.79609271250000002</v>
       </c>
       <c r="H11" s="5">
@@ -4295,11 +4291,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="38"/>
-    <col min="2" max="2" width="12.6328125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.36328125" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="38"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4339,10 +4333,10 @@
       <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="33">
         <v>6.1697057375000002</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="29">
         <v>26.711977300000001</v>
       </c>
       <c r="E6" s="30">
@@ -4354,10 +4348,10 @@
       <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="33">
         <v>6.7950501375000014</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="29">
         <v>47.095998512500003</v>
       </c>
       <c r="E7" s="30">
@@ -4369,10 +4363,10 @@
       <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="33">
         <v>6.7948362500000004</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="29">
         <v>47.100811512500002</v>
       </c>
       <c r="E8" s="30">
@@ -4384,10 +4378,10 @@
       <c r="B9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="33">
         <v>6.2440859624999998</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="29">
         <v>38.586125849999988</v>
       </c>
       <c r="E9" s="30">
@@ -4399,10 +4393,10 @@
       <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="33">
         <v>6.3481880500000001</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="29">
         <v>39.604275862500003</v>
       </c>
       <c r="E10" s="30">
@@ -4414,7 +4408,7 @@
       <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="34">
         <v>6.7948178124999998</v>
       </c>
       <c r="D11" s="31">
@@ -4446,10 +4440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E82DCF-ACB4-4573-B551-26FEF839147A}">
-  <dimension ref="A2:Q10"/>
+  <dimension ref="A2:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4573,49 +4567,49 @@
       <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6">
         <v>6.8019247374999994</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6">
         <v>3.6477314624999999</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6">
         <v>11.4921248125</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6">
         <v>3.3317403374999999</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6">
         <v>49.0709284</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6">
         <v>77.901687622070313</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6">
         <v>0.58357352018356323</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6">
         <v>1.5386009216308589</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6">
         <v>0.70353573749999998</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6">
         <v>5.664835E-2</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6">
         <v>62.279582912499997</v>
       </c>
-      <c r="N6" s="34">
+      <c r="N6">
         <v>0.56889972499999997</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6">
         <v>1.1165649999999999E-2</v>
       </c>
-      <c r="P6" s="34">
+      <c r="P6">
         <v>0.43870282500000002</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q6">
         <v>0.49429488750000011</v>
       </c>
     </row>
@@ -4624,49 +4618,49 @@
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7">
         <v>6.8410622375000001</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7">
         <v>3.7643412500000002</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7">
         <v>12.2463460125</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7">
         <v>3.8597496499999999</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7">
         <v>49.083601312500001</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7">
         <v>75.305313110351563</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7">
         <v>0.58070212602615356</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7">
         <v>1.5033029317855831</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7">
         <v>0.9495681250000001</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7">
         <v>5.3758275000000001E-2</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7">
         <v>62.533862487500002</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7">
         <v>0.68058252499999994</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7">
         <v>1.2849575E-2</v>
       </c>
-      <c r="P7" s="35">
+      <c r="P7">
         <v>0.46165331250000002</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7">
         <v>0.49734814999999999</v>
       </c>
     </row>
@@ -4675,49 +4669,49 @@
       <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8">
         <v>6.8487869625000002</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8">
         <v>3.6463918749999999</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8">
         <v>12.1247729</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8">
         <v>3.846536</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8">
         <v>49.072670625000001</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8">
         <v>75.441482543945313</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8">
         <v>0.58275717496871948</v>
       </c>
-      <c r="J8" s="36">
+      <c r="J8">
         <v>1.536573171615601</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8">
         <v>0.88750671250000013</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8">
         <v>5.3821012500000001E-2</v>
       </c>
-      <c r="M8" s="36">
+      <c r="M8">
         <v>62.526385287499991</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8">
         <v>0.63847419999999999</v>
       </c>
-      <c r="O8" s="36">
+      <c r="O8">
         <v>1.2647274999999999E-2</v>
       </c>
-      <c r="P8" s="36">
+      <c r="P8">
         <v>0.48693291249999998</v>
       </c>
-      <c r="Q8" s="36">
+      <c r="Q8">
         <v>0.51769682500000003</v>
       </c>
     </row>
@@ -4726,49 +4720,49 @@
       <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9">
         <v>6.8097071124999982</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9">
         <v>3.5577312249999999</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9">
         <v>11.773524399999999</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9">
         <v>3.4236784999999998</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9">
         <v>49.000402100000002</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9">
         <v>77.551620483398438</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9">
         <v>0.58242005109786987</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9">
         <v>1.5250241756439209</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9">
         <v>0.68631197499999996</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9">
         <v>5.6238912499999988E-2</v>
       </c>
-      <c r="M9" s="37">
+      <c r="M9">
         <v>62.318067637499993</v>
       </c>
-      <c r="N9" s="37">
+      <c r="N9">
         <v>0.56326893749999996</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9">
         <v>1.2896700000000001E-2</v>
       </c>
-      <c r="P9" s="37">
+      <c r="P9">
         <v>0.42225075000000001</v>
       </c>
-      <c r="Q9" s="37">
+      <c r="Q9">
         <v>0.48955779999999999</v>
       </c>
     </row>
@@ -4777,119 +4771,173 @@
       <c r="B10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10">
         <v>6.8630799499999986</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10">
         <v>3.9567044</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10">
         <v>12.650901087499999</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10">
         <v>4.1797051874999998</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10">
         <v>49.158537362499999</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10">
         <v>75.368484497070313</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10">
         <v>0.58012223243713379</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10">
         <v>1.495667457580566</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10">
         <v>0.94102117499999982</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10">
         <v>5.3878412500000007E-2</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10">
         <v>62.5163167125</v>
       </c>
-      <c r="N10" s="38">
+      <c r="N10">
         <v>0.70130887500000005</v>
       </c>
-      <c r="O10" s="38">
+      <c r="O10">
         <v>1.9570424999999999E-2</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10">
         <v>0.43445107500000002</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10">
         <v>0.49144506249999997</v>
       </c>
     </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="18"/>
+      <c r="B11" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="36">
+        <v>6.8782237000000013</v>
+      </c>
+      <c r="D11" s="36">
+        <v>3.9527949374999989</v>
+      </c>
+      <c r="E11" s="36">
+        <v>12.6761035375</v>
+      </c>
+      <c r="F11" s="36">
+        <v>4.1669741250000003</v>
+      </c>
+      <c r="G11" s="36">
+        <v>49.271688787499997</v>
+      </c>
+      <c r="H11" s="36">
+        <v>75.534103393554688</v>
+      </c>
+      <c r="I11" s="36">
+        <v>0.58266514539718628</v>
+      </c>
+      <c r="J11" s="36">
+        <v>1.5293678045272829</v>
+      </c>
+      <c r="K11" s="36">
+        <v>0.93398606250000005</v>
+      </c>
+      <c r="L11" s="36">
+        <v>5.4051712500000001E-2</v>
+      </c>
+      <c r="M11" s="36">
+        <v>62.495690324999998</v>
+      </c>
+      <c r="N11" s="36">
+        <v>0.6763206625</v>
+      </c>
+      <c r="O11" s="36">
+        <v>2.1499987500000001E-2</v>
+      </c>
+      <c r="P11" s="36">
+        <v>0.46468751250000001</v>
+      </c>
+      <c r="Q11" s="36">
+        <v>0.51082403749999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="35"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C10">
+  <conditionalFormatting sqref="C5:C11">
     <cfRule type="top10" dxfId="50" priority="127" rank="1"/>
     <cfRule type="top10" dxfId="49" priority="128" rank="2"/>
     <cfRule type="top10" dxfId="48" priority="129" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D10">
+  <conditionalFormatting sqref="D5:D11">
     <cfRule type="top10" dxfId="47" priority="130" rank="1"/>
     <cfRule type="top10" dxfId="46" priority="131" rank="2"/>
     <cfRule type="top10" dxfId="45" priority="132" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E10">
+  <conditionalFormatting sqref="E5:E11">
     <cfRule type="top10" dxfId="44" priority="133" rank="1"/>
     <cfRule type="top10" dxfId="43" priority="134" rank="2"/>
     <cfRule type="top10" dxfId="42" priority="135" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F10">
+  <conditionalFormatting sqref="F5:F11">
     <cfRule type="top10" dxfId="41" priority="136" rank="1"/>
     <cfRule type="top10" dxfId="40" priority="137" rank="2"/>
     <cfRule type="top10" dxfId="39" priority="138" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G10">
+  <conditionalFormatting sqref="G5:G11">
     <cfRule type="top10" dxfId="38" priority="139" rank="1"/>
     <cfRule type="top10" dxfId="37" priority="140" rank="2"/>
     <cfRule type="top10" dxfId="36" priority="141" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H10">
+  <conditionalFormatting sqref="H5:H11">
     <cfRule type="top10" dxfId="35" priority="142" rank="1"/>
     <cfRule type="top10" dxfId="34" priority="143" rank="2"/>
     <cfRule type="top10" dxfId="33" priority="144" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I10">
+  <conditionalFormatting sqref="I5:I11">
     <cfRule type="top10" dxfId="32" priority="145" rank="1"/>
     <cfRule type="top10" dxfId="31" priority="146" rank="2"/>
     <cfRule type="top10" dxfId="30" priority="147" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J10">
+  <conditionalFormatting sqref="J5:J11">
     <cfRule type="top10" dxfId="29" priority="148" rank="1"/>
     <cfRule type="top10" dxfId="28" priority="149" rank="2"/>
     <cfRule type="top10" dxfId="27" priority="150" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K10">
+  <conditionalFormatting sqref="K5:K11">
     <cfRule type="top10" dxfId="26" priority="151" rank="1"/>
     <cfRule type="top10" dxfId="25" priority="152" rank="2"/>
     <cfRule type="top10" dxfId="24" priority="153" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L10">
+  <conditionalFormatting sqref="L5:L11">
     <cfRule type="top10" dxfId="23" priority="154" bottom="1" rank="1"/>
     <cfRule type="top10" dxfId="22" priority="155" bottom="1" rank="2"/>
     <cfRule type="top10" dxfId="21" priority="156" bottom="1" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M10">
+  <conditionalFormatting sqref="M5:M11">
     <cfRule type="top10" dxfId="20" priority="157" rank="1"/>
     <cfRule type="top10" dxfId="19" priority="158" rank="2"/>
     <cfRule type="top10" dxfId="18" priority="159" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N10">
+  <conditionalFormatting sqref="N5:N11">
     <cfRule type="top10" dxfId="17" priority="160" rank="1"/>
     <cfRule type="top10" dxfId="16" priority="161" rank="2"/>
     <cfRule type="top10" dxfId="15" priority="162" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P5:P10">
+  <conditionalFormatting sqref="P5:P11">
     <cfRule type="top10" dxfId="14" priority="163" rank="1"/>
     <cfRule type="top10" dxfId="13" priority="164" rank="2"/>
     <cfRule type="top10" dxfId="12" priority="165" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5:Q10">
+  <conditionalFormatting sqref="Q5:Q11">
     <cfRule type="top10" dxfId="11" priority="166" rank="1"/>
     <cfRule type="top10" dxfId="10" priority="167" rank="2"/>
     <cfRule type="top10" dxfId="9" priority="168" rank="3"/>
@@ -4908,10 +4956,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="38"/>
-    <col min="2" max="2" width="12.6328125" style="38" customWidth="1"/>
-    <col min="3" max="5" width="9.36328125" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="38"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4954,7 +5000,7 @@
       <c r="C6" s="4">
         <v>3.6477314624999999</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6">
         <v>0.70353573749999998</v>
       </c>
       <c r="E6" s="5">
@@ -4969,7 +5015,7 @@
       <c r="C7" s="4">
         <v>3.7643412500000002</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7">
         <v>0.9495681250000001</v>
       </c>
       <c r="E7" s="5">
@@ -4984,7 +5030,7 @@
       <c r="C8" s="4">
         <v>3.6463918749999999</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8">
         <v>0.88750671250000013</v>
       </c>
       <c r="E8" s="5">
@@ -4999,7 +5045,7 @@
       <c r="C9" s="4">
         <v>3.5577312249999999</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9">
         <v>0.68631197499999996</v>
       </c>
       <c r="E9" s="5">

</xml_diff>